<commit_message>
change model due to requirement
</commit_message>
<xml_diff>
--- a/testData.xlsx
+++ b/testData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e7994c8fb138f2f6/Documents/CU_Year3/projects/ShiftWorkScheduler/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="144" documentId="11_F25DC773A252ABDACC1048B8C99C52105BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0A450F2-9CAE-4192-BBC8-B7005DDF99A7}"/>
+  <xr:revisionPtr revIDLastSave="214" documentId="11_F25DC773A252ABDACC1048B8C99C52105BDE58F2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3C0C069E-D936-4EBE-86E7-3A0DF10D15FF}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,14 +26,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="44">
   <si>
     <t>ฉาย</t>
   </si>
   <si>
-    <t>วัชรพงษ์</t>
-  </si>
-  <si>
     <t>สุรศักดิ์</t>
   </si>
   <si>
@@ -48,9 +46,6 @@
     <t>วันหยุด</t>
   </si>
   <si>
-    <t>คนขับ</t>
-  </si>
-  <si>
     <t>คนขับทดแทน</t>
   </si>
   <si>
@@ -142,6 +137,27 @@
   </si>
   <si>
     <t>อุดม</t>
+  </si>
+  <si>
+    <t>วัชระพงษ์</t>
+  </si>
+  <si>
+    <t>คนขับเย็น</t>
+  </si>
+  <si>
+    <t>คนขับวันหยุด</t>
+  </si>
+  <si>
+    <t>เดือนที่หยุด</t>
+  </si>
+  <si>
+    <t>มาฆะบูชา</t>
+  </si>
+  <si>
+    <t>วันจักรี</t>
+  </si>
+  <si>
+    <t>วันสงกรานต์</t>
   </si>
 </sst>
 </file>
@@ -462,164 +478,249 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF719DEC-4CB2-4AD4-BD92-E9609B71AE89}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="265" zoomScaleNormal="265" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.85546875" customWidth="1"/>
-    <col min="3" max="3" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="6" width="27.42578125" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="1" max="2" width="18" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" customWidth="1"/>
+    <col min="5" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="8" width="27.42578125" customWidth="1"/>
+    <col min="9" max="9" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
         <v>6</v>
       </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>11</v>
-      </c>
       <c r="F1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="G1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>13</v>
+      <c r="B2">
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>37</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>23</v>
+        <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
+      </c>
+      <c r="I3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H4" t="s">
+        <v>21</v>
+      </c>
+      <c r="I4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>6</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
         <v>14</v>
       </c>
-      <c r="C3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="H5" t="s">
+        <v>22</v>
+      </c>
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>37</v>
+      </c>
+      <c r="G6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>14</v>
+      </c>
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
         <v>16</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H7" t="s">
         <v>24</v>
       </c>
-      <c r="G3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="I7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>15</v>
+      </c>
+      <c r="B8">
+        <v>4</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
         <v>17</v>
       </c>
-      <c r="F4" t="s">
+      <c r="H8" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="I8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
         <v>18</v>
       </c>
-      <c r="F5" t="s">
+      <c r="H9" t="s">
         <v>26</v>
       </c>
-      <c r="G5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="E6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="E9" t="s">
-        <v>22</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>38</v>
+      <c r="I9" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>